<commit_message>
Save scan data and refactor frnt end settings page
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Defsecone\DSEC360-Backend\DSEC\base\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\defsecone project\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37E52D-01FB-41D0-933D-9909C6307AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532FA0FE-9917-442D-92DF-CEF74C15B15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>NetworkDevices</t>
+  </si>
+  <si>
+    <t>MSSQL_2019</t>
   </si>
 </sst>
 </file>
@@ -425,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,7 +983,7 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
implemented for the mssql and maria db
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\defsecone project\DSEC360-\backend\DSEC\scan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Z_PROJECT\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC110305-2603-4B66-8310-4522195B586F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8ECC01-A106-485C-9A89-BC2BB18C0FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$67</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -57,19 +57,28 @@
     <t>Ubuntu_Linux_24.04_LTS_Benchmark_v1.0.0</t>
   </si>
   <si>
-    <t>Microsoft SQL Server 2019 Benchmark v1.5.0</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server 2017 Benchmark v1.3.0</t>
-  </si>
-  <si>
-    <t>Microsoft SQL Server 2016 Benchmark v1.4.0</t>
-  </si>
-  <si>
     <t>Windows 10 Stand-alone</t>
   </si>
   <si>
     <t>Oracle</t>
+  </si>
+  <si>
+    <t>Maria Server v10_6</t>
+  </si>
+  <si>
+    <t>Maria Server v10_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft SQL Server 2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft SQL Server 2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft SQL Server 2019 </t>
+  </si>
+  <si>
+    <t>Microsoft SQL Server 2022</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -432,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -443,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -465,7 +474,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -476,7 +485,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -487,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -498,9 +507,42 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the maria db and mysql for csv,name_changed
</commit_message>
<xml_diff>
--- a/backend/DSEC/scan/data/Configuration_Audit.xlsx
+++ b/backend/DSEC/scan/data/Configuration_Audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Z_PROJECT\DSEC360-\backend\DSEC\scan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8ECC01-A106-485C-9A89-BC2BB18C0FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F699BF7A-9C3C-46E9-8E66-84B2846FD8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,12 +63,6 @@
     <t>Oracle</t>
   </si>
   <si>
-    <t>Maria Server v10_6</t>
-  </si>
-  <si>
-    <t>Maria Server v10_11</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microsoft SQL Server 2016 </t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Microsoft SQL Server 2022</t>
+  </si>
+  <si>
+    <t>MariaDB 10_6</t>
+  </si>
+  <si>
+    <t>MariaDB 10_11</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -496,7 +496,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -507,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -518,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -529,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -540,7 +540,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>

</xml_diff>